<commit_message>
ajuste de testes após mudanças de funcionalidades ARV
</commit_message>
<xml_diff>
--- a/src/test/resources/armazenador/IncluirCNPJs_Ofertas_App.xlsx
+++ b/src/test/resources/armazenador/IncluirCNPJs_Ofertas_App.xlsx
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="Channels">Channels!$A$1:$A$3</definedName>
     <definedName name="Dados">#REF!</definedName>
-    <definedName name="Plans">Plans!$A$1:$A$77</definedName>
+    <definedName name="Plans">Plans!$A$1:$A$7</definedName>
     <definedName name="Sheet2list">Sheet2!$B$1:$B$3</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Inclusão / Exclusão de Relacionamento de CNPJs x Ofertas</t>
   </si>
@@ -77,237 +77,27 @@
     <t>EXCLUSAO</t>
   </si>
   <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Plano Flex</t>
+  </si>
+  <si>
+    <t>TX_FLEX_00,01_7</t>
+  </si>
+  <si>
+    <t>Teste_Gabi</t>
+  </si>
+  <si>
+    <t>Na Medida</t>
+  </si>
+  <si>
+    <t>Teste Na Medida</t>
+  </si>
+  <si>
     <t>Todo Dia</t>
   </si>
   <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>FLEX</t>
-  </si>
-  <si>
-    <t>PLANO NOVO</t>
-  </si>
-  <si>
-    <t>Teste_Gabi</t>
-  </si>
-  <si>
-    <t>Plano Flex</t>
-  </si>
-  <si>
-    <t>Na Medida</t>
-  </si>
-  <si>
-    <t>PLANO 60</t>
-  </si>
-  <si>
-    <t>PLANO 41</t>
-  </si>
-  <si>
-    <t>PLANO 42</t>
-  </si>
-  <si>
-    <t>PLANO 43</t>
-  </si>
-  <si>
-    <t>PLANO 44</t>
-  </si>
-  <si>
-    <t>PLANO 45</t>
-  </si>
-  <si>
-    <t>PLANO 39</t>
-  </si>
-  <si>
-    <t>PLANO 14</t>
-  </si>
-  <si>
-    <t>PLANO 18</t>
-  </si>
-  <si>
-    <t>PLANO 19</t>
-  </si>
-  <si>
-    <t>PLANO 21</t>
-  </si>
-  <si>
-    <t>PLANO 22</t>
-  </si>
-  <si>
-    <t>PLANO 23</t>
-  </si>
-  <si>
-    <t>PLANO 24</t>
-  </si>
-  <si>
-    <t>PLANO 25</t>
-  </si>
-  <si>
-    <t>PLANO 26</t>
-  </si>
-  <si>
-    <t>PLANO 27</t>
-  </si>
-  <si>
-    <t>PLANO 28</t>
-  </si>
-  <si>
-    <t>PLANO 29</t>
-  </si>
-  <si>
-    <t>PLANO 30</t>
-  </si>
-  <si>
-    <t>PLANO 31</t>
-  </si>
-  <si>
-    <t>PLANO 32</t>
-  </si>
-  <si>
-    <t>PLANO 33</t>
-  </si>
-  <si>
-    <t>PLANO 34</t>
-  </si>
-  <si>
-    <t>PLANO 35</t>
-  </si>
-  <si>
-    <t>PLANO 36</t>
-  </si>
-  <si>
-    <t>PLANO 37</t>
-  </si>
-  <si>
-    <t>PLANO 38</t>
-  </si>
-  <si>
-    <t>PLANO 46</t>
-  </si>
-  <si>
-    <t>PLANO 47</t>
-  </si>
-  <si>
-    <t>PLANO 48</t>
-  </si>
-  <si>
-    <t>PLANO 49</t>
-  </si>
-  <si>
-    <t>PLANO 50</t>
-  </si>
-  <si>
-    <t>PLANO 51</t>
-  </si>
-  <si>
-    <t>PLANO 52</t>
-  </si>
-  <si>
-    <t>PLANO 53</t>
-  </si>
-  <si>
-    <t>PLANO 54</t>
-  </si>
-  <si>
-    <t>PLANO 55</t>
-  </si>
-  <si>
-    <t>PLANO 56</t>
-  </si>
-  <si>
-    <t>PLANO 57</t>
-  </si>
-  <si>
-    <t>PLANO 58</t>
-  </si>
-  <si>
-    <t>PLANO 59</t>
-  </si>
-  <si>
-    <t>PLANO 61</t>
-  </si>
-  <si>
-    <t>PLANO 62</t>
-  </si>
-  <si>
-    <t>PLANO 63</t>
-  </si>
-  <si>
-    <t>PLANO 64</t>
-  </si>
-  <si>
-    <t>PLANO 65</t>
-  </si>
-  <si>
-    <t>PLANO 66</t>
-  </si>
-  <si>
-    <t>PLANO 67</t>
-  </si>
-  <si>
-    <t>PLANO 68</t>
-  </si>
-  <si>
-    <t>PLANO 69</t>
-  </si>
-  <si>
-    <t>PLANO 70</t>
-  </si>
-  <si>
-    <t>PLANO 71</t>
-  </si>
-  <si>
-    <t>PLANO 72</t>
-  </si>
-  <si>
-    <t>PLANO 73</t>
-  </si>
-  <si>
-    <t>PLANO 74</t>
-  </si>
-  <si>
-    <t>PLANO 75</t>
-  </si>
-  <si>
-    <t>PLANO 76</t>
-  </si>
-  <si>
-    <t>PLANO 04</t>
-  </si>
-  <si>
-    <t>PLANO 05</t>
-  </si>
-  <si>
-    <t>PLANO 06</t>
-  </si>
-  <si>
-    <t>PLANO 07</t>
-  </si>
-  <si>
-    <t>PLANO 09</t>
-  </si>
-  <si>
-    <t>PLANO 11</t>
-  </si>
-  <si>
-    <t>PLANO 12</t>
-  </si>
-  <si>
-    <t>PLANO 13</t>
-  </si>
-  <si>
-    <t>PLANO 15</t>
-  </si>
-  <si>
-    <t>PLANO 16</t>
-  </si>
-  <si>
-    <t>PLANO 17</t>
-  </si>
-  <si>
-    <t>PLANO 20</t>
-  </si>
-  <si>
     <t>PortalECMobileAPP</t>
   </si>
   <si>
@@ -317,10 +107,10 @@
     <t>FrontVendas</t>
   </si>
   <si>
-    <t>28.339.982/0001-60</t>
-  </si>
-  <si>
-    <t>2000496258</t>
+    <t>1015000255</t>
+  </si>
+  <si>
+    <t>12.259.140/0001-68</t>
   </si>
 </sst>
 </file>
@@ -330,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -375,19 +165,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -439,7 +216,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -473,12 +250,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -877,7 +648,7 @@
   <dimension ref="A1:AMK23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -896,14 +667,14 @@
     <row r="1" spans="1:27" s="5" customFormat="1" ht="52.5" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -951,20 +722,20 @@
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="14" t="s">
-        <v>95</v>
+      <c r="A3" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="10">
-        <v>44013</v>
+        <v>44075</v>
       </c>
       <c r="E3" s="10">
-        <v>44418</v>
+        <v>44440</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>12</v>
@@ -973,7 +744,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -1019,7 +790,7 @@
     <row r="8" spans="1:27">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="13"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -1186,8 +957,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1250,7 +1021,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1289,356 +1060,6 @@
     <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1656,17 +1077,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>